<commit_message>
Correction des alt des images 1,2,3 et 4
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
   <si>
     <t>Catégorie</t>
   </si>
@@ -325,13 +325,25 @@
   </si>
   <si>
     <t>quatre images ont le même texte alternatif (légende de l'image fonction alt=</t>
+  </si>
+  <si>
+    <t>Les alt des images sont identique au h3 qui les précédent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la répétition de alt et du h3 qui les précédent font perdre de la crédibilité du site par le bot google </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La fonction alt doit décrire la photo et non donné l'intention de l auteur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changer les alt pour qu'ils soit correct </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -370,20 +382,12 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="9"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="9"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
-      <color theme="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -425,7 +429,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -434,11 +438,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -655,7 +657,7 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -715,370 +717,385 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" t="s">
+    <row r="5" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:26" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:6" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:6" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:6" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1">
+      <c r="A20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="8" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="A21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="5"/>

</xml_diff>